<commit_message>
unify the conception of DataNode, DataTable, Entity.
Former-commit-id: 99b33b5962f5b40d6cbddc2782ab132c8e72c4ec [formerly 5508b87280d57b908bf7c82b09689655524272ab] [formerly 9196299d21d129b3d2bdf0a6b0b6f6facb41e894 [formerly 64a9b4c5f1652cb36a7ae6a5d93387574a73e3ff]]
Former-commit-id: 95d6d11a465bfb55aed9976fff1a899cd3faf2c2 [formerly 11b208b84cdc600c8889c8a781df62e28d97655c]
Former-commit-id: 51dcf6213aecef90e822b5670b398e5794126c78
Former-commit-id: f079258ab980d3cac31367192fa2e539651a480e
</commit_message>
<xml_diff>
--- a/Bin/Server/DataConfig/Excel/Buff.xlsx
+++ b/Bin/Server/DataConfig/Excel/Buff.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Desktop/NoahGameFrame/_Out/Server/NFDataCfg/Excel_Ini/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpp\ArkGameFrame\Bin\Server\DataConfig\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27520" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="27525" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Property1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataNode" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
@@ -27,8 +27,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -130,8 +130,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -142,6 +142,11 @@
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -341,13 +346,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -681,29 +689,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.625" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="22.625" customWidth="1"/>
+    <col min="5" max="5" width="17.125" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="18.375" customWidth="1"/>
+    <col min="9" max="9" width="19.375" customWidth="1"/>
+    <col min="10" max="10" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -927,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="81" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
@@ -1024,9 +1032,10 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A7"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:J6 B7:J7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A7" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:J6 B7:J7" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add a new tools for processing excel files
Former-commit-id: f13caf72a1850475f4a19e97fce81ede2da52a8c
Former-commit-id: 8e6a5b6138f9b8c4e970ddee0e6ddb1a28f80242
</commit_message>
<xml_diff>
--- a/Bin/Server/DataConfig/Excel/Buff.xlsx
+++ b/Bin/Server/DataConfig/Excel/Buff.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpp\ArkGameFrame\Bin\Server\DataConfig\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\ArkGameFrame\Bin\Server\DataConfig\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="27525" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="27528" windowHeight="17532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataNode" sheetId="1" r:id="rId1"/>
@@ -694,24 +694,24 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="11.625" customWidth="1"/>
-    <col min="3" max="3" width="17.125" customWidth="1"/>
-    <col min="4" max="4" width="22.625" customWidth="1"/>
-    <col min="5" max="5" width="17.125" customWidth="1"/>
-    <col min="6" max="6" width="20.5" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
-    <col min="8" max="8" width="18.375" customWidth="1"/>
-    <col min="9" max="9" width="19.375" customWidth="1"/>
-    <col min="10" max="10" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -743,7 +743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -775,7 +775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -871,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="86.4" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
@@ -967,7 +967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
fix FileProcessor bugs use new path in ElementModule
Former-commit-id: 2fab39fd3dc40c1c34e2a4c20cfbf420403539dd [formerly 727c783d6a5b6987be0e88cc9d1d696bdf0f96fd] [formerly 828005cdfe6fdf7ddb1e496fa6225b77c1d7b305 [formerly 3a7520246b18476c897fabdec54184d5033b9b00]]
Former-commit-id: 926ada9632107bdd0e98df5207647c98ebe9234c [formerly 481e8662e4f8284c622b525137fc0c91308fbc25]
Former-commit-id: d6e61f96f9858889e1e95f1032c2090f87600a35
Former-commit-id: 29746256ece2931585e0a6dd3ebb5d9429faaf08
</commit_message>
<xml_diff>
--- a/Bin/Server/DataConfig/Excel/Buff.xlsx
+++ b/Bin/Server/DataConfig/Excel/Buff.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\ArkGameFrame\Bin\Server\DataConfig\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpp\ARK\Bin\Server\DataConfig\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="27528" windowHeight="17532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="27525" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataNode" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Id</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>Buff_1</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>Buff_2</t>
@@ -131,6 +128,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0_ "/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -301,7 +301,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -341,7 +341,10 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -694,24 +697,24 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="11.625" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="22.625" customWidth="1"/>
+    <col min="5" max="5" width="17.125" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="18.375" customWidth="1"/>
+    <col min="9" max="9" width="19.375" customWidth="1"/>
+    <col min="10" max="10" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -743,7 +746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -775,7 +778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -807,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
@@ -839,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -871,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
@@ -903,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
@@ -935,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" ht="86.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="81" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
@@ -967,44 +970,44 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-      <c r="I9" s="5">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>28</v>
+      <c r="B10" s="13">
+        <v>1</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1034,13 +1037,13 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A7" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:J6 B7:J7" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:A7" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:J7" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>